<commit_message>
Modificación de la memoria
</commit_message>
<xml_diff>
--- a/Plantilla Autoevaluación Practica 3 SI.xlsx
+++ b/Plantilla Autoevaluación Practica 3 SI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - UNIVERSIDAD DE HUELVA\UHU\2019-2020\SISTEMAS INTELIGENTES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igor_\Desktop\Simulacion-covid-19-Supermercado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{02011B15-CE90-2348-B7E1-64AF3FE09114}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2F1E3B10-2551-4AB7-8A91-D867AD5B3970}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9750B2-3FE0-44C6-BE0C-70B7A356302D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A938FD81-2322-B247-9103-89EC5582B1DB}"/>
   </bookViews>
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98B1762-DC99-DF49-8944-4AC94F66497A}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1157,10 +1157,10 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       <c r="C38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="9" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>